<commit_message>
fix: various fixes for usability
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Weranest\Documents\UiPath\IgnitisHW_Performer\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4867C6B8-4580-4304-9A89-F8BC11D0CC67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EA59B13-F956-47AE-8083-8C41E8AB6663}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17235" yWindow="7200" windowWidth="18660" windowHeight="6525" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="58">
   <si>
     <t>Name</t>
   </si>
@@ -165,38 +165,102 @@
     <t>MasterfilePath</t>
   </si>
   <si>
-    <t>RPA001_IgnitisHW_SongsPerBand</t>
-  </si>
-  <si>
-    <t>RPA001_IgnitisHW_MasterfilePath</t>
-  </si>
-  <si>
     <t>RPA001_IgnitisHW_Queue</t>
   </si>
   <si>
-    <t>RPA001_IgnitisHW_EmailTo</t>
-  </si>
-  <si>
-    <t>RPA001_IgnitisHW_WorkFolderPath</t>
-  </si>
-  <si>
     <t>MaxVideoLength</t>
   </si>
   <si>
-    <t>RPA001_IgnitisHW_MaxVideoLength</t>
-  </si>
-  <si>
     <t>WorkFolderPath</t>
   </si>
   <si>
     <t>EmailTo</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 00:06:00 </t>
+  </si>
+  <si>
+    <t>MaxVideosParsed</t>
+  </si>
+  <si>
+    <t>Path to the "Grupės.xlsx" file</t>
+  </si>
+  <si>
+    <t>Path to the work folder used to store files (the program will create a new folder inside the selected path and will not interact with any other file present in the path)</t>
+  </si>
+  <si>
+    <t>Email address that is to be used as the recipient of the zip files at the end of the process</t>
+  </si>
+  <si>
+    <t>Number of songs to be included in each search results final output</t>
+  </si>
+  <si>
+    <r>
+      <t>Maximum videos parsed for each band. Higher numbers are possibly more prone to breaking and take longer, but are more likely to return the correct amount of videos requested (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>not in use currently</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>REQUIRED format</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>hh:mm:ss</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve"> ///// Maximum length of videos to be included in the final output. When parsed, videos with higher values than the one here will not be parsed</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -220,6 +284,18 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -238,10 +314,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -252,8 +329,10 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -619,7 +698,7 @@
         <v>24</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>22</v>
@@ -2814,15 +2893,16 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="31.85546875" customWidth="1"/>
-    <col min="2" max="2" width="30.140625" customWidth="1"/>
+    <col min="2" max="2" width="70.5703125" customWidth="1"/>
     <col min="3" max="3" width="60.28515625" customWidth="1"/>
-    <col min="4" max="26" width="65.42578125" customWidth="1"/>
+    <col min="4" max="4" width="180.42578125" customWidth="1"/>
+    <col min="5" max="26" width="65.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -2863,45 +2943,62 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D2" t="s">
         <v>53</v>
-      </c>
-      <c r="B2" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1">
       <c r="A3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B3" s="6"/>
+      <c r="D3" t="s">
         <v>54</v>
-      </c>
-      <c r="B3" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1">
       <c r="A4" t="s">
         <v>44</v>
       </c>
-      <c r="B4" t="s">
-        <v>46</v>
+      <c r="B4">
+        <v>5</v>
+      </c>
+      <c r="D4" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1">
       <c r="A5" t="s">
         <v>45</v>
       </c>
-      <c r="B5" t="s">
-        <v>47</v>
+      <c r="D5" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1">
       <c r="A6" t="s">
+        <v>47</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A7" t="s">
         <v>51</v>
       </c>
-      <c r="B6" s="5" t="s">
-        <v>52</v>
+      <c r="B7">
+        <v>100</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>56</v>
       </c>
     </row>
-    <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
@@ -3898,5 +3995,6 @@
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fix: fixed minor issues and documentation
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Weranest\Documents\UiPath\IgnitisHW_Performer\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EA59B13-F956-47AE-8083-8C41E8AB6663}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B699B3A8-1926-4B7C-941D-7239811E151A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="61">
   <si>
     <t>Name</t>
   </si>
@@ -181,9 +181,6 @@
   </si>
   <si>
     <t>MaxVideosParsed</t>
-  </si>
-  <si>
-    <t>Path to the "Grupės.xlsx" file</t>
   </si>
   <si>
     <t>Path to the work folder used to store files (the program will create a new folder inside the selected path and will not interact with any other file present in the path)</t>
@@ -254,6 +251,18 @@
       </rPr>
       <t xml:space="preserve"> ///// Maximum length of videos to be included in the final output. When parsed, videos with higher values than the one here will not be parsed</t>
     </r>
+  </si>
+  <si>
+    <t>C:\Users\Weranest\Documents\IgnitisHW</t>
+  </si>
+  <si>
+    <t>weranest@gmail.com</t>
+  </si>
+  <si>
+    <t>C:\Users\Weranest\Desktop\Grupės.xlsx</t>
+  </si>
+  <si>
+    <t>Path to the "Grupės.xlsx" file. The ending needs to contain "Grupės.xlsx"</t>
   </si>
 </sst>
 </file>
@@ -2893,7 +2902,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -2945,17 +2954,22 @@
       <c r="A2" t="s">
         <v>48</v>
       </c>
+      <c r="B2" t="s">
+        <v>57</v>
+      </c>
       <c r="D2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1">
       <c r="A3" t="s">
         <v>49</v>
       </c>
-      <c r="B3" s="6"/>
+      <c r="B3" s="6" t="s">
+        <v>58</v>
+      </c>
       <c r="D3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1">
@@ -2966,15 +2980,18 @@
         <v>5</v>
       </c>
       <c r="D4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1">
       <c r="A5" t="s">
         <v>45</v>
       </c>
+      <c r="B5" t="s">
+        <v>59</v>
+      </c>
       <c r="D5" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1">
@@ -2985,7 +3002,7 @@
         <v>50</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
@@ -2996,7 +3013,7 @@
         <v>100</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
@@ -3994,7 +4011,10 @@
     <row r="1000" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
+  <hyperlinks>
+    <hyperlink ref="B3" r:id="rId1" xr:uid="{68B0B1C7-BB31-4AB2-B7E3-226DA6644205}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>